<commit_message>
Update crosswalk parameter files
Last update of crosswalk parameter files
</commit_message>
<xml_diff>
--- a/Crosswalk_2012/Crosswalk_Algae_Weeds.xlsx
+++ b/Crosswalk_2012/Crosswalk_Algae_Weeds.xlsx
@@ -217,9 +217,6 @@
     <t>OR_SR_1706010407_02_103329</t>
   </si>
   <si>
-    <t>OR_WS_170900120201_02_104554</t>
-  </si>
-  <si>
     <t>Pollutant</t>
   </si>
   <si>
@@ -311,6 +308,9 @@
   </si>
   <si>
     <t>OR_LK_1709001202_02_107245</t>
+  </si>
+  <si>
+    <t>OR_WS_170900120201_02_104554.1</t>
   </si>
 </sst>
 </file>
@@ -1129,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,25 +1150,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1179,16 +1179,16 @@
         <v>174</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1199,19 +1199,19 @@
         <v>173</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1222,19 +1222,19 @@
         <v>173</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1245,19 +1245,19 @@
         <v>173</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1268,16 +1268,16 @@
         <v>173</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>63</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1288,19 +1288,19 @@
         <v>173</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1311,16 +1311,16 @@
         <v>173</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1331,16 +1331,16 @@
         <v>173</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1351,16 +1351,16 @@
         <v>174</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1371,16 +1371,16 @@
         <v>174</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1391,16 +1391,16 @@
         <v>174</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1411,16 +1411,16 @@
         <v>174</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1431,16 +1431,16 @@
         <v>174</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1451,16 +1451,16 @@
         <v>175</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1471,16 +1471,16 @@
         <v>175</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1491,19 +1491,19 @@
         <v>175</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1514,16 +1514,16 @@
         <v>175</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1534,16 +1534,16 @@
         <v>175</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1554,16 +1554,16 @@
         <v>174</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1574,16 +1574,16 @@
         <v>173</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1594,16 +1594,16 @@
         <v>174</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1614,16 +1614,16 @@
         <v>174</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1634,16 +1634,16 @@
         <v>175</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1654,19 +1654,19 @@
         <v>175</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1677,16 +1677,16 @@
         <v>175</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1697,16 +1697,16 @@
         <v>173</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1717,16 +1717,16 @@
         <v>173</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1737,16 +1737,16 @@
         <v>174</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1757,16 +1757,16 @@
         <v>174</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1777,16 +1777,16 @@
         <v>174</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1797,16 +1797,16 @@
         <v>173</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1817,16 +1817,16 @@
         <v>173</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1837,16 +1837,16 @@
         <v>175</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1857,16 +1857,16 @@
         <v>175</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1877,16 +1877,16 @@
         <v>173</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>59</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1897,16 +1897,16 @@
         <v>173</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1917,16 +1917,16 @@
         <v>174</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1937,16 +1937,16 @@
         <v>174</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1957,16 +1957,16 @@
         <v>174</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1977,16 +1977,16 @@
         <v>173</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1997,16 +1997,16 @@
         <v>173</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2017,19 +2017,19 @@
         <v>174</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2040,16 +2040,16 @@
         <v>174</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2060,16 +2060,16 @@
         <v>174</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2080,16 +2080,16 @@
         <v>174</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2100,16 +2100,16 @@
         <v>174</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2120,16 +2120,16 @@
         <v>174</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2140,16 +2140,16 @@
         <v>174</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2160,16 +2160,16 @@
         <v>174</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2180,16 +2180,16 @@
         <v>174</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2200,16 +2200,16 @@
         <v>174</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2220,19 +2220,19 @@
         <v>174</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2243,16 +2243,16 @@
         <v>174</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2263,16 +2263,16 @@
         <v>174</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2283,16 +2283,16 @@
         <v>174</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2303,16 +2303,16 @@
         <v>174</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2323,16 +2323,16 @@
         <v>174</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2343,16 +2343,16 @@
         <v>174</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2363,16 +2363,16 @@
         <v>174</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>57</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2383,16 +2383,16 @@
         <v>174</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2403,16 +2403,16 @@
         <v>174</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2423,16 +2423,16 @@
         <v>174</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2443,16 +2443,16 @@
         <v>174</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2463,19 +2463,19 @@
         <v>174</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2486,16 +2486,16 @@
         <v>174</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2506,19 +2506,19 @@
         <v>174</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D67" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2529,16 +2529,16 @@
         <v>174</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2549,16 +2549,16 @@
         <v>174</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2569,16 +2569,16 @@
         <v>175</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2589,16 +2589,16 @@
         <v>175</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2609,19 +2609,19 @@
         <v>175</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F72" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G72" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2632,16 +2632,16 @@
         <v>174</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>52</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2652,16 +2652,16 @@
         <v>175</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2672,16 +2672,16 @@
         <v>175</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2692,16 +2692,16 @@
         <v>175</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2712,16 +2712,16 @@
         <v>175</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2732,16 +2732,16 @@
         <v>175</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2752,19 +2752,19 @@
         <v>175</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D79" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2775,19 +2775,19 @@
         <v>175</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2798,19 +2798,19 @@
         <v>174</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2821,16 +2821,16 @@
         <v>175</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2841,19 +2841,19 @@
         <v>175</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D83" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2861,11 +2861,10 @@
         <v>90006</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H84"/>
   <sortState ref="A2:H85">
     <sortCondition ref="A1"/>
   </sortState>

</xml_diff>